<commit_message>
import excel data in app & notebook
</commit_message>
<xml_diff>
--- a/content.xlsx
+++ b/content.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28829"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\egos\Mon Drive\ORDI\PYTHON3\JV\WB7 EAPP tool\EEPA-tool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33484504-33F6-4257-83CC-DCB56BD14D53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E1BFB48-F490-4307-ADD2-DACBE38BA57A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30624" yWindow="0" windowWidth="30912" windowHeight="16656" activeTab="1" xr2:uid="{B32870CE-8A9E-4DDD-8F12-75D0127A347E}"/>
+    <workbookView xWindow="28836" yWindow="3708" windowWidth="14796" windowHeight="12120" activeTab="2" xr2:uid="{B32870CE-8A9E-4DDD-8F12-75D0127A347E}"/>
   </bookViews>
   <sheets>
     <sheet name="Part A" sheetId="1" r:id="rId1"/>
     <sheet name="Part B" sheetId="2" r:id="rId2"/>
+    <sheet name="Titlle" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="30">
   <si>
     <t>Pillar 1: Institutional Readiness</t>
   </si>
@@ -204,6 +205,18 @@
   </si>
   <si>
     <t>content</t>
+  </si>
+  <si>
+    <t>Pillar 3: Operational Readiness</t>
+  </si>
+  <si>
+    <t>This pillar assesses progress towards developing and using service and administration infrastructure required for a program.</t>
+  </si>
+  <si>
+    <t>Pillar 4: Insurance Market Readiness</t>
+  </si>
+  <si>
+    <t>This pillar assesses your progress towards implementing the most appropriate risk financing options for the program.</t>
   </si>
 </sst>
 </file>
@@ -278,45 +291,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <fgColor theme="0"/>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -649,7 +624,7 @@
   <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1032,10 +1007,57 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDF2360F-6F61-40A9-9A8C-B24CA87A9037}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B80A1FDD-0AD3-4361-B4BA-4BFBC65F510B}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>